<commit_message>
Update code to accept date query
</commit_message>
<xml_diff>
--- a/query_config.xlsx
+++ b/query_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SorinoSK\School\Internship\Work\IoT\Intern-IoT-Data-Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CD043A-31A9-4698-9EDC-77C2DFDFD4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30AD74B0-2E25-4DC4-B348-7F17B09F0FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
   </bookViews>
   <sheets>
     <sheet name="units_to_query" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="179">
   <si>
     <t>5kW - Unit 9</t>
   </si>
@@ -597,6 +597,15 @@
   </si>
   <si>
     <t>p2dcv</t>
+  </si>
+  <si>
+    <t>From Date</t>
+  </si>
+  <si>
+    <t>To Date</t>
+  </si>
+  <si>
+    <t>"To Date" will collect up to this date that means up to 2359 of the day before</t>
   </si>
 </sst>
 </file>
@@ -643,7 +652,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -756,11 +765,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -789,6 +820,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1103,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6952B871-99E0-F341-BE0D-6033E27DBDAB}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1115,10 +1158,12 @@
     <col min="2" max="2" width="35.875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.125" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.875" style="1"/>
+    <col min="5" max="5" width="21.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="86.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="86.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -1131,24 +1176,40 @@
       <c r="D1" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="8" cm="1">
-        <f t="array" ref="A2">INDEX(data_sheet!$A$2:$A$21,MATCH(1,(data_sheet!$B$2:$B$21=units_to_query!B2)*(data_sheet!$C$2:$C$21=units_to_query!D2),0))</f>
-        <v>71</v>
+        <f t="array" ref="A2">INDEX(data_sheet!$A$2:$A$100,MATCH(1,(data_sheet!$B$2:$B$100=units_to_query!B2)*(data_sheet!$C$2:$C$100=units_to_query!D2),0))</f>
+        <v>72</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C2" s="9">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>19</v>
       </c>
+      <c r="E2" s="16">
+        <v>44888</v>
+      </c>
+      <c r="F2" s="17">
+        <v>45260</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>178</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -1180,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAAFFF8-797D-4622-8EAF-B6B9DA77F942}">
   <dimension ref="A1:A200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1201,77 +1262,77 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>22</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>56</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>153</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>54</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>113</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>125</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>117</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>157</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>171</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -1281,106 +1342,158 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>48</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-    </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
+      <c r="A28" s="12" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
+      <c r="A29" s="12" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
+      <c r="A30" s="12" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
+      <c r="A31" s="12" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
+      <c r="A32" s="12" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
+      <c r="A33" s="12" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
+      <c r="A34" s="12" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
+      <c r="A35" s="12" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
+      <c r="A36" s="12" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
+      <c r="A37" s="12" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
+      <c r="A38" s="12" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
+      <c r="A39" s="12" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
+      <c r="A40" s="12" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
+      <c r="A41" s="12" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
+      <c r="A42" s="12" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
+      <c r="A43" s="12" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
+      <c r="A44" s="12" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
+      <c r="A45" s="12" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
+      <c r="A46" s="12" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
+      <c r="A47" s="12" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
+      <c r="A48" s="12" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
+      <c r="A49" s="12" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>

</xml_diff>

<commit_message>
change write order to be ascending
</commit_message>
<xml_diff>
--- a/query_config.xlsx
+++ b/query_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SorinoSK\School\Internship\Work\IoT\Intern-IoT-Data-Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30AD74B0-2E25-4DC4-B348-7F17B09F0FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794552BE-5A2B-4E26-A8D6-B7F9CAFEE000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
   </bookViews>
   <sheets>
     <sheet name="units_to_query" sheetId="1" r:id="rId1"/>
@@ -1149,7 +1149,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1198,10 +1198,10 @@
         <v>19</v>
       </c>
       <c r="E2" s="16">
-        <v>44888</v>
+        <v>44887</v>
       </c>
       <c r="F2" s="17">
-        <v>45260</v>
+        <v>44918</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>178</v>

</xml_diff>

<commit_message>
update to date to 2359 and update README
</commit_message>
<xml_diff>
--- a/query_config.xlsx
+++ b/query_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SorinoSK\School\Internship\Work\IoT\Intern-IoT-Data-Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794552BE-5A2B-4E26-A8D6-B7F9CAFEE000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAC911F-B623-4690-9EEE-7804A72106F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
   </bookViews>
@@ -1149,7 +1149,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1198,10 +1198,10 @@
         <v>19</v>
       </c>
       <c r="E2" s="16">
-        <v>44887</v>
+        <v>44880</v>
       </c>
       <c r="F2" s="17">
-        <v>44918</v>
+        <v>44881</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>178</v>

</xml_diff>

<commit_message>
Update Null Date Bug
</commit_message>
<xml_diff>
--- a/query_config.xlsx
+++ b/query_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SorinoSK\School\Internship\Work\IoT\Intern-IoT-Data-Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B9DF04-C8C3-4A95-8DD7-E4A182A1C575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D248B7E-3F84-41B6-AF2B-40CECDAD6070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="345" windowWidth="21600" windowHeight="11295" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
+    <workbookView xWindow="8145" yWindow="1425" windowWidth="21600" windowHeight="11295" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
   </bookViews>
   <sheets>
     <sheet name="units_to_query" sheetId="1" r:id="rId1"/>
@@ -813,7 +813,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -827,6 +826,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1145,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6952B871-99E0-F341-BE0D-6033E27DBDAB}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1173,33 +1175,29 @@
       <c r="D1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="8" cm="1">
         <f t="array" ref="A2">INDEX(data_sheet!$A$2:$A$100,MATCH(1,(data_sheet!$B$2:$B$100=units_to_query!B2)*(data_sheet!$C$2:$C$100=units_to_query!D2),0))</f>
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C2" s="9">
-        <v>140</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="16">
-        <v>44880</v>
-      </c>
-      <c r="F2" s="17">
-        <v>44881</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1250,697 +1248,697 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="11" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="11" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="11" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="11" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="11" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="11" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="11" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="11" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="11" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="11" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
+      <c r="A37" s="11" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="11" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="11" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="11" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="11" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="11" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="11" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
+      <c r="A44" s="11" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
+      <c r="A45" s="11" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
+      <c r="A46" s="11" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
+      <c r="A47" s="11" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
+      <c r="A48" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
+      <c r="A49" s="11" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
+      <c r="A50" s="11"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
+      <c r="A51" s="11"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
+      <c r="A52" s="11"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
+      <c r="A53" s="11"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="12"/>
+      <c r="A54" s="11"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
+      <c r="A55" s="11"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
+      <c r="A56" s="11"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="12"/>
+      <c r="A57" s="11"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
+      <c r="A58" s="11"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="12"/>
+      <c r="A59" s="11"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
+      <c r="A60" s="11"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="12"/>
+      <c r="A61" s="11"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="12"/>
+      <c r="A62" s="11"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="12"/>
+      <c r="A63" s="11"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="12"/>
+      <c r="A64" s="11"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="12"/>
+      <c r="A65" s="11"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="12"/>
+      <c r="A66" s="11"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="12"/>
+      <c r="A67" s="11"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="12"/>
+      <c r="A68" s="11"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="12"/>
+      <c r="A69" s="11"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="12"/>
+      <c r="A70" s="11"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="12"/>
+      <c r="A71" s="11"/>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="12"/>
+      <c r="A72" s="11"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="12"/>
+      <c r="A73" s="11"/>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="12"/>
+      <c r="A74" s="11"/>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="12"/>
+      <c r="A75" s="11"/>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="12"/>
+      <c r="A76" s="11"/>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="12"/>
+      <c r="A77" s="11"/>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="12"/>
+      <c r="A78" s="11"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="12"/>
+      <c r="A79" s="11"/>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="12"/>
+      <c r="A80" s="11"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="12"/>
+      <c r="A81" s="11"/>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="12"/>
+      <c r="A82" s="11"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="12"/>
+      <c r="A83" s="11"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="12"/>
+      <c r="A84" s="11"/>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="12"/>
+      <c r="A85" s="11"/>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="12"/>
+      <c r="A86" s="11"/>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="12"/>
+      <c r="A87" s="11"/>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="12"/>
+      <c r="A88" s="11"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="12"/>
+      <c r="A89" s="11"/>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="12"/>
+      <c r="A90" s="11"/>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="12"/>
+      <c r="A91" s="11"/>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="12"/>
+      <c r="A92" s="11"/>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="12"/>
+      <c r="A93" s="11"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="12"/>
+      <c r="A94" s="11"/>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="12"/>
+      <c r="A95" s="11"/>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="12"/>
+      <c r="A96" s="11"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="12"/>
+      <c r="A97" s="11"/>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="12"/>
+      <c r="A98" s="11"/>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="12"/>
+      <c r="A99" s="11"/>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="12"/>
+      <c r="A100" s="11"/>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="12"/>
+      <c r="A101" s="11"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="12"/>
+      <c r="A102" s="11"/>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="12"/>
+      <c r="A103" s="11"/>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="12"/>
+      <c r="A104" s="11"/>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="12"/>
+      <c r="A105" s="11"/>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="12"/>
+      <c r="A106" s="11"/>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="12"/>
+      <c r="A107" s="11"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="12"/>
+      <c r="A108" s="11"/>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="12"/>
+      <c r="A109" s="11"/>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="12"/>
+      <c r="A110" s="11"/>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="12"/>
+      <c r="A111" s="11"/>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="12"/>
+      <c r="A112" s="11"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="12"/>
+      <c r="A113" s="11"/>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="12"/>
+      <c r="A114" s="11"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="12"/>
+      <c r="A115" s="11"/>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="12"/>
+      <c r="A116" s="11"/>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="12"/>
+      <c r="A117" s="11"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="12"/>
+      <c r="A118" s="11"/>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="12"/>
+      <c r="A119" s="11"/>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="12"/>
+      <c r="A120" s="11"/>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="12"/>
+      <c r="A121" s="11"/>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="12"/>
+      <c r="A122" s="11"/>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="12"/>
+      <c r="A123" s="11"/>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="12"/>
+      <c r="A124" s="11"/>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="12"/>
+      <c r="A125" s="11"/>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="12"/>
+      <c r="A126" s="11"/>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="12"/>
+      <c r="A127" s="11"/>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="12"/>
+      <c r="A128" s="11"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="12"/>
+      <c r="A129" s="11"/>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="12"/>
+      <c r="A130" s="11"/>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="12"/>
+      <c r="A131" s="11"/>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="12"/>
+      <c r="A132" s="11"/>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="12"/>
+      <c r="A133" s="11"/>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="12"/>
+      <c r="A134" s="11"/>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="12"/>
+      <c r="A135" s="11"/>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="12"/>
+      <c r="A136" s="11"/>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="12"/>
+      <c r="A137" s="11"/>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="12"/>
+      <c r="A138" s="11"/>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="12"/>
+      <c r="A139" s="11"/>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="12"/>
+      <c r="A140" s="11"/>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="12"/>
+      <c r="A141" s="11"/>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="12"/>
+      <c r="A142" s="11"/>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="12"/>
+      <c r="A143" s="11"/>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="12"/>
+      <c r="A144" s="11"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="12"/>
+      <c r="A145" s="11"/>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="12"/>
+      <c r="A146" s="11"/>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="12"/>
+      <c r="A147" s="11"/>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="12"/>
+      <c r="A148" s="11"/>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="12"/>
+      <c r="A149" s="11"/>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="12"/>
+      <c r="A150" s="11"/>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="12"/>
+      <c r="A151" s="11"/>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="12"/>
+      <c r="A152" s="11"/>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="12"/>
+      <c r="A153" s="11"/>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="12"/>
+      <c r="A154" s="11"/>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="12"/>
+      <c r="A155" s="11"/>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="12"/>
+      <c r="A156" s="11"/>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="12"/>
+      <c r="A157" s="11"/>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="12"/>
+      <c r="A158" s="11"/>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="12"/>
+      <c r="A159" s="11"/>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="12"/>
+      <c r="A160" s="11"/>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="12"/>
+      <c r="A161" s="11"/>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="12"/>
+      <c r="A162" s="11"/>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="12"/>
+      <c r="A163" s="11"/>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="12"/>
+      <c r="A164" s="11"/>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="12"/>
+      <c r="A165" s="11"/>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="12"/>
+      <c r="A166" s="11"/>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="12"/>
+      <c r="A167" s="11"/>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="12"/>
+      <c r="A168" s="11"/>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="12"/>
+      <c r="A169" s="11"/>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" s="12"/>
+      <c r="A170" s="11"/>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="12"/>
+      <c r="A171" s="11"/>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="12"/>
+      <c r="A172" s="11"/>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" s="12"/>
+      <c r="A173" s="11"/>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="12"/>
+      <c r="A174" s="11"/>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="12"/>
+      <c r="A175" s="11"/>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="12"/>
+      <c r="A176" s="11"/>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="12"/>
+      <c r="A177" s="11"/>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="12"/>
+      <c r="A178" s="11"/>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="12"/>
+      <c r="A179" s="11"/>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="12"/>
+      <c r="A180" s="11"/>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="12"/>
+      <c r="A181" s="11"/>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" s="12"/>
+      <c r="A182" s="11"/>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="12"/>
+      <c r="A183" s="11"/>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184" s="12"/>
+      <c r="A184" s="11"/>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="12"/>
+      <c r="A185" s="11"/>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="12"/>
+      <c r="A186" s="11"/>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="12"/>
+      <c r="A187" s="11"/>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="12"/>
+      <c r="A188" s="11"/>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="12"/>
+      <c r="A189" s="11"/>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="12"/>
+      <c r="A190" s="11"/>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" s="12"/>
+      <c r="A191" s="11"/>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="12"/>
+      <c r="A192" s="11"/>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="12"/>
+      <c r="A193" s="11"/>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" s="12"/>
+      <c r="A194" s="11"/>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="12"/>
+      <c r="A195" s="11"/>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="12"/>
+      <c r="A196" s="11"/>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="12"/>
+      <c r="A197" s="11"/>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="12"/>
+      <c r="A198" s="11"/>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="12"/>
+      <c r="A199" s="11"/>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="13"/>
+      <c r="A200" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add features for invalid date range.
</commit_message>
<xml_diff>
--- a/query_config.xlsx
+++ b/query_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SorinoSK\School\Internship\Work\IoT\Intern-IoT-Data-Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D248B7E-3F84-41B6-AF2B-40CECDAD6070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B478F31-C302-4F54-BF2C-7EB050D61AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8145" yWindow="1425" windowWidth="21600" windowHeight="11295" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
   </bookViews>
   <sheets>
     <sheet name="units_to_query" sheetId="1" r:id="rId1"/>
@@ -1148,7 +1148,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1191,13 +1191,17 @@
         <v>8</v>
       </c>
       <c r="C2" s="9">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16"/>
+      <c r="E2" s="15">
+        <v>45056</v>
+      </c>
+      <c r="F2" s="16">
+        <v>45050</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>